<commit_message>
CS_06_02_CO versión final completo
Después de revisión de coordinación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1515" windowWidth="19440" windowHeight="11640" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1515" windowWidth="19440" windowHeight="11640" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="69">
   <si>
     <t>FICHA</t>
   </si>
@@ -94,9 +94,6 @@
     <t>CS_06_02_CO</t>
   </si>
   <si>
-    <t>Conocer cómo vivían las comunidades humanas antes de invención de la escritura nos permite comprender el proceso de evolución cultural en los primeros tiempos de la humanidad</t>
-  </si>
-  <si>
     <t>Educación Básica Secundaria</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Refuerza tu aprendizaje: Los orígenes del ser humano</t>
   </si>
   <si>
-    <t>Amplía tus conocimientos: Periodos de la historia de América y Colombia</t>
-  </si>
-  <si>
     <t>si</t>
   </si>
   <si>
@@ -233,6 +227,15 @@
   </si>
   <si>
     <t>La Prehistoria</t>
+  </si>
+  <si>
+    <t>Conocer cómo vivían las comunidades humanas antes de la invención de la escritura nos permite comprender el proceso de evolución cultural en los primeros tiempos de la humanidad</t>
+  </si>
+  <si>
+    <t>Refuerza el aprendizaje: El Mesolítico</t>
+  </si>
+  <si>
+    <t>Etapas de la Prehistoria</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1723,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1754,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1762,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1778,7 +1781,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1800,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,25 +1836,29 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
+      <c r="A2" t="str">
+        <f>[1]Hoja1!A2283</f>
+        <v>1° ESO</v>
+      </c>
+      <c r="B2" t="str">
+        <f>[1]Hoja1!B2283</f>
+        <v>CS</v>
+      </c>
+      <c r="C2" t="str">
+        <f>[1]Hoja1!C2283</f>
+        <v>Introducción a la historia y la prehistoria</v>
+      </c>
+      <c r="D2" t="str">
+        <f>[1]Hoja1!D2283</f>
+        <v>El proceso de hominización</v>
+      </c>
+      <c r="E2" t="str">
+        <f>[1]Hoja1!E2283</f>
+        <v>CS_07_07</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
@@ -1859,25 +1866,25 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>[1]Hoja1!A2283</f>
-        <v>1° ESO</v>
+      <c r="A3">
+        <f>[1]Hoja1!A13422</f>
+        <v>5</v>
       </c>
       <c r="B3" t="str">
-        <f>[1]Hoja1!B2283</f>
-        <v>CS</v>
+        <f>[1]Hoja1!B13422</f>
+        <v>MS</v>
       </c>
       <c r="C3" t="str">
-        <f>[1]Hoja1!C2283</f>
-        <v>Introducción a la historia y la prehistoria</v>
+        <f>[1]Hoja1!C13422</f>
+        <v>La prehistoria</v>
       </c>
       <c r="D3" t="str">
-        <f>[1]Hoja1!D2283</f>
-        <v>El proceso de hominización</v>
+        <f>[1]Hoja1!D13422</f>
+        <v>Identifica a nuestros antepasados</v>
       </c>
       <c r="E3" t="str">
-        <f>[1]Hoja1!E2283</f>
-        <v>CS_07_07</v>
+        <f>[1]Hoja1!E13422</f>
+        <v>MS_3C_07</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1885,48 +1892,48 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>[1]Hoja1!A13422</f>
+        <f>[1]Hoja1!A13424</f>
         <v>5</v>
       </c>
       <c r="B4" t="str">
-        <f>[1]Hoja1!B13422</f>
+        <f>[1]Hoja1!B13424</f>
         <v>MS</v>
       </c>
       <c r="C4" t="str">
-        <f>[1]Hoja1!C13422</f>
+        <f>[1]Hoja1!C13424</f>
         <v>La prehistoria</v>
       </c>
       <c r="D4" t="str">
-        <f>[1]Hoja1!D13422</f>
-        <v>Identifica a nuestros antepasados</v>
+        <f>[1]Hoja1!D13424</f>
+        <v>El paleolítico</v>
       </c>
       <c r="E4" t="str">
-        <f>[1]Hoja1!E13422</f>
+        <f>[1]Hoja1!E13424</f>
         <v>MS_3C_07</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>[1]Hoja1!A13424</f>
+        <f>[1]Hoja1!A13425</f>
         <v>5</v>
       </c>
       <c r="B5" t="str">
-        <f>[1]Hoja1!B13424</f>
+        <f>[1]Hoja1!B13425</f>
         <v>MS</v>
       </c>
       <c r="C5" t="str">
-        <f>[1]Hoja1!C13424</f>
+        <f>[1]Hoja1!C13425</f>
         <v>La prehistoria</v>
       </c>
       <c r="D5" t="str">
-        <f>[1]Hoja1!D13424</f>
-        <v>El paleolítico</v>
+        <f>[1]Hoja1!D13425</f>
+        <v>Identifica las características del paleolítico</v>
       </c>
       <c r="E5" t="str">
-        <f>[1]Hoja1!E13424</f>
+        <f>[1]Hoja1!E13425</f>
         <v>MS_3C_07</v>
       </c>
       <c r="F5">
@@ -1934,28 +1941,23 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>[1]Hoja1!A13425</f>
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f>[1]Hoja1!B13425</f>
-        <v>MS</v>
-      </c>
-      <c r="C6" t="str">
-        <f>[1]Hoja1!C13425</f>
-        <v>La prehistoria</v>
-      </c>
-      <c r="D6" t="str">
-        <f>[1]Hoja1!D13425</f>
-        <v>Identifica las características del paleolítico</v>
-      </c>
-      <c r="E6" t="str">
-        <f>[1]Hoja1!E13425</f>
-        <v>MS_3C_07</v>
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2228,7 +2230,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,32 +2252,32 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -2283,10 +2285,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -2314,7 +2316,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,11 +2342,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>'RECURSOS APROVECHADOS'!$D$2</f>
-        <v>Reconoce los cambios del neolítico y la edad de los metales</v>
+        <f>'RECURSOS APROVECHADOS'!D2</f>
+        <v>El proceso de hominización</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,22 +2355,21 @@
       </c>
       <c r="B3" t="str">
         <f>'RECURSOS APROVECHADOS'!D3</f>
-        <v>El proceso de hominización</v>
+        <v>Identifica a nuestros antepasados</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <f>'RECURSOS APROVECHADOS'!D4</f>
-        <v>Identifica a nuestros antepasados</v>
+      <c r="B4" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2376,11 +2377,11 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f>'RECURSOS NUEVOS'!$A$2</f>
-        <v>Refuerza tu aprendizaje: Los orígenes del ser humano</v>
+        <f>'RECURSOS APROVECHADOS'!D4</f>
+        <v>El paleolítico</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,10 +2390,10 @@
       </c>
       <c r="B6" t="str">
         <f>'RECURSOS APROVECHADOS'!D5</f>
-        <v>El paleolítico</v>
+        <v>Identifica las características del paleolítico</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,11 +2401,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f>'RECURSOS APROVECHADOS'!D6</f>
-        <v>Identifica las características del paleolítico</v>
+        <f>'RECURSOS NUEVOS'!$A$3</f>
+        <v>Refuerza el aprendizaje: El Mesolítico</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2412,11 +2413,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f>'RECURSOS NUEVOS'!$A$3</f>
-        <v>Amplía tus conocimientos: Periodos de la historia de América y Colombia</v>
+        <f>'RECURSOS APROVECHADOS'!$D$6</f>
+        <v>Reconoce los cambios del neolítico y la edad de los metales</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2429,7 @@
         <v>El neolítico</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2440,7 +2441,7 @@
         <v>Conoce la revolución neolítica</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,7 +2453,7 @@
         <v>Refuerza tu aprendizaje: El neolítico</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2464,7 +2465,7 @@
         <v>El neolítico y la edad de los metales</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,7 +2477,7 @@
         <v>Relaciona conceptos con su período histórico</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2489,7 @@
         <v>El arte en la prehistoria</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2501,7 @@
         <v>Reconoce los distintos monumentos megalíticos</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2512,7 +2513,7 @@
         <v>Refuerza tu aprendizaje: El arte en la prehistoria</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,7 +2525,7 @@
         <v>Competencias: comentario de una obra de arte de la prehistoria</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,7 +2537,7 @@
         <v>Proyecto: análisis de las costumbres del ser humano</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2544,10 +2545,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2555,10 +2556,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2581,10 +2582,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,7 +2594,9 @@
     <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="67.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2632,10 +2635,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -2649,10 +2652,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -2666,10 +2669,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -2683,35 +2686,31 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>33</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="18" t="s">
-        <v>37</v>
-      </c>
+      <c r="D6" s="18"/>
       <c r="E6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -2723,55 +2722,55 @@
         <v>19</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="19" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
@@ -2780,88 +2779,87 @@
         <v>19</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="G10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="E11" s="18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D12" s="18"/>
       <c r="E12" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="H12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -2874,86 +2872,87 @@
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="A18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -2967,10 +2966,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -2984,13 +2983,15 @@
         <v>19</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+        <v>40</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19"/>
@@ -3001,22 +3002,20 @@
         <v>19</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="17"/>
-      <c r="D22" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3024,10 +3023,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -3040,10 +3039,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -3056,32 +3055,37 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3089,13 +3093,13 @@
         <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,10 +3107,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3114,16 +3118,16 @@
         <v>19</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3131,13 +3135,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3145,16 +3149,16 @@
         <v>19</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3162,10 +3166,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
@@ -3179,10 +3183,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
@@ -3196,10 +3200,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
@@ -3213,77 +3217,71 @@
         <v>19</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="19"/>
+      <c r="H35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
+      <c r="E36" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
-      <c r="H36" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="H36" s="16"/>
+      <c r="I36" s="19"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37" s="20"/>
-      <c r="D37" s="21" t="s">
-        <v>40</v>
-      </c>
+      <c r="D37" s="21"/>
       <c r="E37" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="19"/>
+      <c r="H37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>33</v>
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3291,10 +3289,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3302,13 +3303,10 @@
         <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3316,10 +3314,10 @@
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3327,10 +3325,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3338,10 +3336,16 @@
         <v>19</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="H43" t="s">
+        <v>60</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3349,16 +3353,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" t="s">
-        <v>62</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3366,13 +3367,10 @@
         <v>19</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3380,10 +3378,16 @@
         <v>19</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H46" t="s">
+        <v>61</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3391,16 +3395,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H47" t="s">
-        <v>63</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3408,13 +3409,10 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3422,10 +3420,10 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3433,10 +3431,10 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3444,10 +3442,13 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3455,38 +3456,41 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="H52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H53" t="s">
-        <v>64</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="A53" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>34</v>
@@ -3495,49 +3499,49 @@
       <c r="E54" s="21"/>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="19"/>
+      <c r="H54" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="20" t="s">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="I56" s="19" t="s">
-        <v>33</v>
+      <c r="H56" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3545,33 +3549,31 @@
         <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C73" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>29</v>
+      <c r="I73" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste esqueleto CS_06_02_CO y otros...
Corrección de mayúsculas en títulos de recursos aprovechados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="71">
   <si>
     <t>FICHA</t>
   </si>
@@ -196,33 +196,12 @@
     <t>Identifica a nuestros antepasados</t>
   </si>
   <si>
-    <t>Identifica las características del Paleolítico</t>
-  </si>
-  <si>
     <t>Conoce la revolución neolítica</t>
   </si>
   <si>
-    <t>Refuerza el aprendizaje: El Neolítico</t>
-  </si>
-  <si>
-    <t>El Neolítico y la Edad de los Metales</t>
-  </si>
-  <si>
-    <t>Relaciona conceptos con su periodo histórico</t>
-  </si>
-  <si>
-    <t>Arte y religión en la Edad de Piedra</t>
-  </si>
-  <si>
     <t>Reconoce los distintos monumentos megalíticos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: El arte en la Prehistoria</t>
-  </si>
-  <si>
-    <t>Competencias: comentario de una obra de arte de la Prehistoria</t>
-  </si>
-  <si>
     <t>Proyecto: análisis de las costumbres del ser humano</t>
   </si>
   <si>
@@ -236,6 +215,33 @@
   </si>
   <si>
     <t>Etapas de la Prehistoria</t>
+  </si>
+  <si>
+    <t>El paleolítico</t>
+  </si>
+  <si>
+    <t>Identifica las características del paleolítico</t>
+  </si>
+  <si>
+    <t>El neolítico</t>
+  </si>
+  <si>
+    <t>Refuerza el aprendizaje: El neolítico</t>
+  </si>
+  <si>
+    <t>El neolítico y la edad de los metales</t>
+  </si>
+  <si>
+    <t>Arte y religión en la edad de piedra</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El arte en la prehistoria</t>
+  </si>
+  <si>
+    <t>Relaciona conceptos con su período histórico</t>
+  </si>
+  <si>
+    <t>Competencias: comentario de una obra de arte de la prehistoria</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1741,7 +1747,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,7 +1763,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,7 +2269,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -2584,8 +2590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,7 +2641,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>32</v>
@@ -2652,7 +2658,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>33</v>
@@ -2669,7 +2675,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>32</v>
@@ -2686,7 +2692,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="18" t="s">
@@ -2705,7 +2711,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="18"/>
@@ -2722,7 +2728,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -2743,7 +2749,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="21"/>
@@ -2762,7 +2768,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="21"/>
@@ -2779,7 +2785,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="21"/>
@@ -2800,7 +2806,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
@@ -2819,7 +2825,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18"/>
@@ -2882,7 +2888,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>31</v>
@@ -2921,7 +2927,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>31</v>
@@ -3012,7 +3018,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>28</v>
@@ -3082,7 +3088,7 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>31</v>
@@ -3124,7 +3130,7 @@
         <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>31</v>
@@ -3155,7 +3161,7 @@
         <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>31</v>
@@ -3227,7 +3233,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="16" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I35" s="19" t="s">
         <v>31</v>
@@ -3267,7 +3273,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
       <c r="H37" s="16" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="I37" s="19" t="s">
         <v>31</v>
@@ -3342,7 +3348,7 @@
         <v>36</v>
       </c>
       <c r="H43" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>31</v>
@@ -3384,7 +3390,7 @@
         <v>34</v>
       </c>
       <c r="H46" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>31</v>
@@ -3462,7 +3468,7 @@
         <v>34</v>
       </c>
       <c r="H52" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>31</v>
@@ -3500,7 +3506,7 @@
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
       <c r="H54" s="16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>31</v>
@@ -3521,7 +3527,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Y va la última
CS_06_02_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CS_06_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1515" windowWidth="19440" windowHeight="11640" tabRatio="729" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="3405" yWindow="1515" windowWidth="19440" windowHeight="11640" tabRatio="729" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="70">
   <si>
     <t>FICHA</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Mapa conceptual</t>
-  </si>
-  <si>
-    <t>Reconoce los cambios del Neolítico y la Edad de los Metales</t>
   </si>
   <si>
     <t>Identifica a nuestros antepasados</t>
@@ -753,7 +750,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -798,6 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1705,7 +1703,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1730,7 +1728,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1746,7 +1744,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2086,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
@@ -2247,7 +2245,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -2299,7 +2297,7 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2566,10 +2564,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
+      <selection activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,7 +2617,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>32</v>
@@ -2636,7 +2634,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>33</v>
@@ -2653,7 +2651,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>32</v>
@@ -2670,7 +2668,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="18" t="s">
@@ -2689,7 +2687,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="18"/>
@@ -2706,7 +2704,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -2727,7 +2725,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="21"/>
@@ -2746,7 +2744,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="21"/>
@@ -2763,7 +2761,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="21"/>
@@ -2773,7 +2771,7 @@
         <v>34</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>31</v>
@@ -2784,7 +2782,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
@@ -2803,7 +2801,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18"/>
@@ -2866,7 +2864,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>31</v>
@@ -2905,7 +2903,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>31</v>
@@ -2996,7 +2994,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>28</v>
@@ -3066,7 +3064,7 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>31</v>
@@ -3108,7 +3106,7 @@
         <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>31</v>
@@ -3139,7 +3137,7 @@
         <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>31</v>
@@ -3211,7 +3209,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I35" s="19" t="s">
         <v>31</v>
@@ -3251,7 +3249,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
       <c r="H37" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I37" s="19" t="s">
         <v>31</v>
@@ -3326,7 +3324,7 @@
         <v>36</v>
       </c>
       <c r="H43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>31</v>
@@ -3368,7 +3366,7 @@
         <v>34</v>
       </c>
       <c r="H46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>31</v>
@@ -3446,7 +3444,7 @@
         <v>34</v>
       </c>
       <c r="H52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>31</v>
@@ -3484,7 +3482,7 @@
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
       <c r="H54" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>31</v>
@@ -3505,7 +3503,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>31</v>
@@ -3545,20 +3543,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C73" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I73" s="19" t="s">
-        <v>31</v>
-      </c>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="5"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>